<commit_message>
Small bug fixing and editing other methods
</commit_message>
<xml_diff>
--- a/example/GRAFS_project_example.xlsx
+++ b/example/GRAFS_project_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faustega\Documents\These\isterre-dynamic-modeling\grafs-e-project\grafs-e\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174F66BA-A498-42AB-936C-D50184D7AEFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3528AEEF-4BDF-416E-9C4E-749860798B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16530" yWindow="-15870" windowWidth="25440" windowHeight="15270" activeTab="4" xr2:uid="{092E5AC7-17CB-4282-9989-CDCB089F75B9}"/>
+    <workbookView xWindow="16530" yWindow="-15870" windowWidth="25440" windowHeight="15270" activeTab="3" xr2:uid="{092E5AC7-17CB-4282-9989-CDCB089F75B9}"/>
   </bookViews>
   <sheets>
     <sheet name="crops" sheetId="1" r:id="rId1"/>
@@ -1034,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9008F097-1A19-4A13-A439-D292DC31E615}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1260,7 +1260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{986D1BE3-7A15-4223-93AE-9AB753B07534}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Minor updates. Docs is created in another directory.
</commit_message>
<xml_diff>
--- a/example/GRAFS_project_example.xlsx
+++ b/example/GRAFS_project_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faustega\Documents\These\isterre-dynamic-modeling\grafs-e-project\grafs-e\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3528AEEF-4BDF-416E-9C4E-749860798B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB09F746-07E3-4945-8A38-2A830F5A0970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16530" yWindow="-15870" windowWidth="25440" windowHeight="15270" activeTab="3" xr2:uid="{092E5AC7-17CB-4282-9989-CDCB089F75B9}"/>
+    <workbookView xWindow="16530" yWindow="-15870" windowWidth="25440" windowHeight="15270" xr2:uid="{092E5AC7-17CB-4282-9989-CDCB089F75B9}"/>
   </bookViews>
   <sheets>
     <sheet name="crops" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
   <si>
     <t>Culture</t>
   </si>
@@ -91,18 +91,6 @@
     <t>BGN</t>
   </si>
   <si>
-    <t>Fan coef a</t>
-  </si>
-  <si>
-    <t>Fan coef b</t>
-  </si>
-  <si>
-    <t>Carbon allocation to grain (%)</t>
-  </si>
-  <si>
-    <t>Carbon allocation to straw (%)</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
@@ -112,9 +100,6 @@
     <t>Maize</t>
   </si>
   <si>
-    <t>Main production</t>
-  </si>
-  <si>
     <t>Livestock</t>
   </si>
   <si>
@@ -221,6 +206,12 @@
   </si>
   <si>
     <t>Meat of pig with the bone fresh or chilled</t>
+  </si>
+  <si>
+    <t>Harvest Index</t>
+  </si>
+  <si>
+    <t>Main Production</t>
   </si>
 </sst>
 </file>
@@ -630,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973E28D2-5D19-4409-920F-79B00DDA2ABC}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -641,17 +632,16 @@
     <col min="1" max="1" width="23.6328125" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="19.1796875" customWidth="1"/>
-    <col min="4" max="4" width="18.36328125" customWidth="1"/>
-    <col min="5" max="5" width="18.7265625" customWidth="1"/>
-    <col min="6" max="7" width="20.36328125" customWidth="1"/>
+    <col min="4" max="4" width="26.54296875" customWidth="1"/>
+    <col min="5" max="5" width="31.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -663,33 +653,24 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -701,33 +682,24 @@
         <v>0</v>
       </c>
       <c r="F2" s="4">
-        <v>40.200000000000003</v>
+        <v>0</v>
       </c>
       <c r="G2" s="4">
-        <v>41.827100000000002</v>
+        <v>0</v>
       </c>
       <c r="H2" s="4">
         <v>0</v>
       </c>
       <c r="I2" s="4">
-        <v>0</v>
-      </c>
-      <c r="J2" s="4">
-        <v>0</v>
-      </c>
-      <c r="K2" s="4">
-        <v>0.34399999999999997</v>
-      </c>
-      <c r="L2" s="4">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -739,33 +711,24 @@
         <v>0</v>
       </c>
       <c r="F3" s="4">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="G3" s="4">
-        <v>42.311399999999999</v>
+        <v>0</v>
       </c>
       <c r="H3" s="4">
         <v>0</v>
       </c>
       <c r="I3" s="4">
-        <v>0</v>
-      </c>
-      <c r="J3" s="4">
-        <v>0</v>
-      </c>
-      <c r="K3" s="4">
-        <v>0.378</v>
-      </c>
-      <c r="L3" s="4">
-        <v>2.8000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
@@ -777,33 +740,24 @@
         <v>0</v>
       </c>
       <c r="F4" s="4">
-        <v>33.1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="4">
-        <v>29.4</v>
+        <v>0</v>
       </c>
       <c r="H4" s="4">
         <v>0</v>
       </c>
       <c r="I4" s="4">
-        <v>0</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0</v>
-      </c>
-      <c r="K4" s="4">
-        <v>0.35699999999999998</v>
-      </c>
-      <c r="L4" s="4">
-        <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -815,33 +769,24 @@
         <v>0</v>
       </c>
       <c r="F5" s="4">
-        <v>42.6</v>
+        <v>0</v>
       </c>
       <c r="G5" s="4">
-        <v>36.299999999999997</v>
+        <v>0</v>
       </c>
       <c r="H5" s="4">
         <v>0</v>
       </c>
       <c r="I5" s="4">
-        <v>0</v>
-      </c>
-      <c r="J5" s="4">
-        <v>0</v>
-      </c>
-      <c r="K5" s="4">
-        <v>0.36899999999999999</v>
-      </c>
-      <c r="L5" s="4">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>5</v>
@@ -853,33 +798,24 @@
         <v>125</v>
       </c>
       <c r="F6" s="4">
-        <v>39.6</v>
+        <v>0</v>
       </c>
       <c r="G6" s="4">
-        <v>40.5794</v>
+        <v>0</v>
       </c>
       <c r="H6" s="4">
         <v>0</v>
       </c>
       <c r="I6" s="4">
-        <v>0</v>
-      </c>
-      <c r="J6" s="4">
-        <v>0</v>
-      </c>
-      <c r="K6" s="4">
-        <v>0</v>
-      </c>
-      <c r="L6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>8</v>
@@ -891,36 +827,27 @@
         <v>0</v>
       </c>
       <c r="F7" s="4">
-        <v>47.571100000000001</v>
+        <v>0.7</v>
       </c>
       <c r="G7" s="4">
-        <v>7.1375000000000002</v>
+        <v>1.01</v>
       </c>
       <c r="H7" s="4">
-        <v>0.7</v>
+        <v>1.3</v>
       </c>
       <c r="I7" s="4">
-        <v>1.01</v>
-      </c>
-      <c r="J7" s="4">
-        <v>1.3</v>
-      </c>
-      <c r="K7" s="4">
-        <v>0</v>
-      </c>
-      <c r="L7" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D8" s="4">
         <v>0</v>
@@ -929,25 +856,16 @@
         <v>150</v>
       </c>
       <c r="F8" s="4">
-        <v>44.618899999999996</v>
+        <v>0.77</v>
       </c>
       <c r="G8" s="4">
-        <v>7.7354000000000003</v>
+        <v>-0.49</v>
       </c>
       <c r="H8" s="4">
-        <v>0.77</v>
+        <v>1.7</v>
       </c>
       <c r="I8" s="4">
-        <v>-0.49</v>
-      </c>
-      <c r="J8" s="4">
-        <v>1.7</v>
-      </c>
-      <c r="K8" s="4">
-        <v>0</v>
-      </c>
-      <c r="L8" s="4">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
@@ -971,13 +889,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1017,12 +935,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1034,7 +952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9008F097-1A19-4A13-A439-D292DC31E615}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -1048,33 +966,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
         <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E2">
         <v>1.95</v>
@@ -1082,16 +1000,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E3">
         <v>1.76</v>
@@ -1099,16 +1017,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E4">
         <v>2.08</v>
@@ -1116,16 +1034,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E5">
         <v>1.52</v>
@@ -1133,16 +1051,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E6">
         <v>1.07</v>
@@ -1150,13 +1068,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -1167,16 +1085,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E8">
         <v>2.0499999999999998</v>
@@ -1184,16 +1102,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E9">
         <v>2.27</v>
@@ -1201,16 +1119,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E10">
         <v>5.3E-3</v>
@@ -1218,16 +1136,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E11">
         <v>2.83</v>
@@ -1235,16 +1153,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E12">
         <v>2.5</v>
@@ -1271,15 +1189,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -1287,7 +1205,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>0.05</v>
@@ -1295,7 +1213,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>0.2</v>
@@ -1303,10 +1221,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>